<commit_message>
skift datastruktur i vl (mastervl og vlListe)
</commit_message>
<xml_diff>
--- a/assets/VL.xlsx
+++ b/assets/VL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebk\makro\p6_data\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8EA345-31A4-4471-A820-3957A74EC331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C7A968-39CC-453A-8837-4AD97776D410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E7DE5B6D-17B1-4BBB-8342-C7DA09B36074}"/>
+    <workbookView xWindow="-120" yWindow="570" windowWidth="29040" windowHeight="16830" xr2:uid="{E7DE5B6D-17B1-4BBB-8342-C7DA09B36074}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2422EC17-15C8-4726-B31A-3667559F39F4}">
   <dimension ref="A1:AU7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>